<commit_message>
Fixed Muskegon DO measurement labels (mg/L & %) to "probe" (NOT LAB!)
</commit_message>
<xml_diff>
--- a/analysis/Verruco Metadata.xlsx
+++ b/analysis/Verruco Metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14280" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -1227,9 +1227,6 @@
     <t>Alk mg/L</t>
   </si>
   <si>
-    <t>DO %</t>
-  </si>
-  <si>
     <t>Turb NTU</t>
   </si>
   <si>
@@ -1260,9 +1257,6 @@
     <t>DO Probe (mg/L)</t>
   </si>
   <si>
-    <t>DO Lab mg/L</t>
-  </si>
-  <si>
     <t>Chl Lab (ug/L)</t>
   </si>
   <si>
@@ -1291,6 +1285,12 @@
   </si>
   <si>
     <t>NH4 ug/L</t>
+  </si>
+  <si>
+    <t>DO probe %</t>
+  </si>
+  <si>
+    <t>DO probe mg/L</t>
   </si>
 </sst>
 </file>
@@ -6693,11 +6693,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU361"/>
+  <dimension ref="A1:AW361"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A189" sqref="A189:XFD189"/>
+      <pane ySplit="1" topLeftCell="A184" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A188" sqref="A188:XFD188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6724,7 +6724,7 @@
     <col min="20" max="20" width="18.83203125" style="4" customWidth="1"/>
     <col min="21" max="41" width="10.83203125" style="4"/>
     <col min="42" max="42" width="10.83203125" style="27"/>
-    <col min="43" max="47" width="10.83203125" style="10"/>
+    <col min="43" max="49" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" s="11" customFormat="1" ht="30">
@@ -6774,7 +6774,7 @@
         <v>394</v>
       </c>
       <c r="P1" s="19" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q1" s="19" t="s">
         <v>391</v>
@@ -6783,13 +6783,13 @@
         <v>395</v>
       </c>
       <c r="S1" s="19" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="T1" s="19" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="U1" s="21" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="V1" s="22" t="s">
         <v>396</v>
@@ -6807,61 +6807,61 @@
         <v>400</v>
       </c>
       <c r="AA1" s="22" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="AB1" s="22" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="AC1" s="22" t="s">
         <v>401</v>
       </c>
       <c r="AD1" s="21" t="s">
-        <v>413</v>
+        <v>423</v>
       </c>
       <c r="AE1" s="21" t="s">
+        <v>422</v>
+      </c>
+      <c r="AF1" s="21" t="s">
         <v>402</v>
       </c>
-      <c r="AF1" s="21" t="s">
-        <v>403</v>
-      </c>
       <c r="AG1" s="19" t="s">
+        <v>416</v>
+      </c>
+      <c r="AH1" s="19" t="s">
+        <v>417</v>
+      </c>
+      <c r="AI1" s="19" t="s">
+        <v>404</v>
+      </c>
+      <c r="AJ1" s="19" t="s">
+        <v>405</v>
+      </c>
+      <c r="AK1" s="19" t="s">
+        <v>406</v>
+      </c>
+      <c r="AL1" s="19" t="s">
+        <v>407</v>
+      </c>
+      <c r="AM1" s="19" t="s">
+        <v>408</v>
+      </c>
+      <c r="AN1" s="19" t="s">
+        <v>409</v>
+      </c>
+      <c r="AO1" s="19" t="s">
+        <v>410</v>
+      </c>
+      <c r="AP1" s="23" t="s">
+        <v>414</v>
+      </c>
+      <c r="AQ1" s="11" t="s">
         <v>418</v>
       </c>
-      <c r="AH1" s="19" t="s">
+      <c r="AR1" s="11" t="s">
         <v>419</v>
       </c>
-      <c r="AI1" s="19" t="s">
-        <v>405</v>
-      </c>
-      <c r="AJ1" s="19" t="s">
-        <v>406</v>
-      </c>
-      <c r="AK1" s="19" t="s">
-        <v>407</v>
-      </c>
-      <c r="AL1" s="19" t="s">
-        <v>408</v>
-      </c>
-      <c r="AM1" s="19" t="s">
-        <v>409</v>
-      </c>
-      <c r="AN1" s="19" t="s">
-        <v>410</v>
-      </c>
-      <c r="AO1" s="19" t="s">
-        <v>411</v>
-      </c>
-      <c r="AP1" s="23" t="s">
-        <v>416</v>
-      </c>
-      <c r="AQ1" s="11" t="s">
-        <v>420</v>
-      </c>
-      <c r="AR1" s="11" t="s">
+      <c r="AS1" s="11" t="s">
         <v>421</v>
-      </c>
-      <c r="AS1" s="11" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="2" spans="1:45" s="3" customFormat="1">

</xml_diff>